<commit_message>
fixed search on multi fields
</commit_message>
<xml_diff>
--- a/uploads/Header for NofaX .xlsx
+++ b/uploads/Header for NofaX .xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awaes Ahmed\Desktop\Nofa Software REquriement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Events_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="20060" windowHeight="7940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Y$1:$Y$1</definedName>
     <definedName name="MDFFund">[1]DataValidation!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Nofa Unique ID</t>
   </si>
@@ -171,9 +171,6 @@
     <t>KRIS REMAUT</t>
   </si>
   <si>
-    <t>ASIF NAZIR</t>
-  </si>
-  <si>
     <t>AWAD TARIQ</t>
   </si>
   <si>
@@ -205,6 +202,15 @@
   </si>
   <si>
     <t>Barcode Number</t>
+  </si>
+  <si>
+    <t>AWAD NAZIR</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>user2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
     <numFmt numFmtId="164" formatCode="[$AED]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1203,7 +1209,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,6 +1226,7 @@
     <xf numFmtId="0" fontId="44" fillId="40" borderId="1" xfId="143" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="143" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="144">
     <cellStyle name="20% - Accent1 2" xfId="16"/>
@@ -1367,8 +1374,36 @@
     <cellStyle name="VerticalTextCenter" xfId="121"/>
     <cellStyle name="Warning Text 2" xfId="122"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1484,23 +1519,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1536,23 +1554,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1731,61 +1732,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AJ1" sqref="AJ1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="106.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="106.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="58.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" s="3" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -1905,7 +1905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41">
       <c r="A3" s="4">
         <v>1001</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -2023,7 +2023,7 @@
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41">
       <c r="A4" s="4">
         <v>1002</v>
       </c>
@@ -2036,19 +2036,21 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -2080,7 +2082,7 @@
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41">
       <c r="A5" s="4">
         <v>1003</v>
       </c>
@@ -2093,19 +2095,21 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -2137,7 +2141,7 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41">
       <c r="A6" s="4">
         <v>1004</v>
       </c>
@@ -2150,12 +2154,12 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2194,7 +2198,7 @@
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41">
       <c r="A7" s="4">
         <v>1005</v>
       </c>
@@ -2207,12 +2211,12 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2251,7 +2255,7 @@
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41">
       <c r="A8" s="4">
         <v>1006</v>
       </c>
@@ -2264,12 +2268,12 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -2309,8 +2313,12 @@
       <c r="AO8" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q4" r:id="rId1"/>
+    <hyperlink ref="Q5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2320,7 +2328,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2332,7 +2340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test feedback 1 fixes
</commit_message>
<xml_diff>
--- a/uploads/Header for NofaX .xlsx
+++ b/uploads/Header for NofaX .xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Events_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awaes Ahmed\Desktop\Nofa Software REquriement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11475"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="20060" windowHeight="7940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Y$1:$Y$1</definedName>
     <definedName name="MDFFund">[1]DataValidation!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>Nofa Unique ID</t>
   </si>
@@ -171,6 +171,9 @@
     <t>KRIS REMAUT</t>
   </si>
   <si>
+    <t>ASIF NAZIR</t>
+  </si>
+  <si>
     <t>AWAD TARIQ</t>
   </si>
   <si>
@@ -202,15 +205,6 @@
   </si>
   <si>
     <t>Barcode Number</t>
-  </si>
-  <si>
-    <t>AWAD NAZIR</t>
-  </si>
-  <si>
-    <t>user1@gmail.com</t>
-  </si>
-  <si>
-    <t>user2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -221,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="[$AED]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,7 +1203,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1226,7 +1220,6 @@
     <xf numFmtId="0" fontId="44" fillId="40" borderId="1" xfId="143" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="143" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="144">
     <cellStyle name="20% - Accent1 2" xfId="16"/>
@@ -1374,36 +1367,8 @@
     <cellStyle name="VerticalTextCenter" xfId="121"/>
     <cellStyle name="Warning Text 2" xfId="122"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1519,6 +1484,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1554,6 +1536,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1732,60 +1731,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AJ1" sqref="AJ1"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="106.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="106.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="58.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" ht="15">
+    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -1905,7 +1905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1001</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -2023,7 +2023,7 @@
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>1002</v>
       </c>
@@ -2036,21 +2036,19 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -2082,7 +2080,7 @@
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>1003</v>
       </c>
@@ -2095,21 +2093,19 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -2141,7 +2137,7 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>1004</v>
       </c>
@@ -2154,12 +2150,12 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2198,7 +2194,7 @@
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>1005</v>
       </c>
@@ -2211,12 +2207,12 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2255,7 +2251,7 @@
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1006</v>
       </c>
@@ -2268,12 +2264,12 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -2313,12 +2309,8 @@
       <c r="AO8" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Q4" r:id="rId1"/>
-    <hyperlink ref="Q5" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2328,7 +2320,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2340,7 +2332,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added dynamic fields in badge layout
</commit_message>
<xml_diff>
--- a/uploads/Header for NofaX .xlsx
+++ b/uploads/Header for NofaX .xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awaes Ahmed\Desktop\Nofa Software REquriement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Events_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="20060" windowHeight="7940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Y$1:$Y$1</definedName>
     <definedName name="MDFFund">[1]DataValidation!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Nofa Unique ID</t>
   </si>
@@ -171,9 +171,6 @@
     <t>KRIS REMAUT</t>
   </si>
   <si>
-    <t>ASIF NAZIR</t>
-  </si>
-  <si>
     <t>AWAD TARIQ</t>
   </si>
   <si>
@@ -205,6 +202,15 @@
   </si>
   <si>
     <t>Barcode Number</t>
+  </si>
+  <si>
+    <t>AWAD NAZIR</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>user2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
     <numFmt numFmtId="164" formatCode="[$AED]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1203,7 +1209,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,6 +1226,7 @@
     <xf numFmtId="0" fontId="44" fillId="40" borderId="1" xfId="143" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="143" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="144">
     <cellStyle name="20% - Accent1 2" xfId="16"/>
@@ -1367,8 +1374,36 @@
     <cellStyle name="VerticalTextCenter" xfId="121"/>
     <cellStyle name="Warning Text 2" xfId="122"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1484,23 +1519,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1536,23 +1554,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1731,61 +1732,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AJ1" sqref="AJ1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="106.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="80.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="106.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="58.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" s="3" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -1905,7 +1905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41">
       <c r="A3" s="4">
         <v>1001</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -2023,7 +2023,7 @@
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41">
       <c r="A4" s="4">
         <v>1002</v>
       </c>
@@ -2036,19 +2036,21 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -2080,7 +2082,7 @@
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41">
       <c r="A5" s="4">
         <v>1003</v>
       </c>
@@ -2093,19 +2095,21 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -2137,7 +2141,7 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41">
       <c r="A6" s="4">
         <v>1004</v>
       </c>
@@ -2150,12 +2154,12 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2194,7 +2198,7 @@
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41">
       <c r="A7" s="4">
         <v>1005</v>
       </c>
@@ -2207,12 +2211,12 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2251,7 +2255,7 @@
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41">
       <c r="A8" s="4">
         <v>1006</v>
       </c>
@@ -2264,12 +2268,12 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -2309,8 +2313,12 @@
       <c r="AO8" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q4" r:id="rId1"/>
+    <hyperlink ref="Q5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2320,7 +2328,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2332,7 +2340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>